<commit_message>
feat : UI_WorkItem 추가
UI_WorkItem 기능이 추가되었습니다.

해당 UI는 WorkTab에 위치해있으며

화면을 터치(클릭) 할 때마다 소지금이 증가하는 이벤트를 업그레이드 합니다.
</commit_message>
<xml_diff>
--- a/I Will be a Rich/Assets/Resources/Data/Excel/StatData.xlsx
+++ b/I Will be a Rich/Assets/Resources/Data/Excel/StatData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LuckyRich_git\I-Will-be-a-Rich\I Will be a Rich\Assets\Resources\Data\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{264F531F-FCF7-4CBB-9741-EB2E0700C484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F213514-CC3D-450F-B2AC-B6A554EE9561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{CD9405CB-3E23-4E0B-9F75-3BA5D4945F52}"/>
   </bookViews>
@@ -86,10 +86,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>touch</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>upgrade00</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -109,6 +105,10 @@
   </si>
   <si>
     <t>maxLevel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>work</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -476,7 +476,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -512,7 +512,7 @@
         <v>10</v>
       </c>
       <c r="H1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
@@ -538,7 +538,7 @@
         <v>13</v>
       </c>
       <c r="H2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
@@ -546,7 +546,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C3">
         <v>10000</v>
@@ -572,7 +572,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>30000</v>
@@ -598,7 +598,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5">
         <v>30001</v>
@@ -624,7 +624,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6">
         <v>30002</v>
@@ -650,7 +650,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7">
         <v>30003</v>

</xml_diff>